<commit_message>
made folders and updated qa gen prompt
</commit_message>
<xml_diff>
--- a/validation/val_20250715_200042.xlsx
+++ b/validation/val_20250715_200042.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dt-summer-corp\RIS-Chatbot\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4747E9BE-A55D-420F-80AA-3F780E421BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A5C88C-B0E0-4B1A-AB06-A51713321B26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{4611F2C1-0F9E-43E4-8EAC-81939FA8E224}"/>
   </bookViews>
@@ -5827,7 +5827,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -5844,7 +5844,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -5895,7 +5895,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -5912,7 +5912,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="348" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -5929,7 +5929,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -5946,7 +5946,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -5963,7 +5963,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -5980,7 +5980,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -6031,7 +6031,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -6065,7 +6065,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -6099,7 +6099,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -6116,7 +6116,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -6252,7 +6252,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -6286,7 +6286,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -6303,7 +6303,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -6320,7 +6320,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -6371,7 +6371,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -6388,7 +6388,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" ht="406" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -6405,7 +6405,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -6422,7 +6422,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -6439,7 +6439,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -6456,7 +6456,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -6507,7 +6507,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -6541,7 +6541,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -6558,7 +6558,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -6626,7 +6626,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -6643,7 +6643,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:5" ht="319" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -6660,7 +6660,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -6677,7 +6677,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -6711,7 +6711,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -6779,7 +6779,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -6847,7 +6847,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -6864,7 +6864,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:5" ht="348" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -6915,7 +6915,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -6932,7 +6932,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -6949,7 +6949,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -6966,7 +6966,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -6983,7 +6983,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -7000,7 +7000,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -7034,7 +7034,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -7085,7 +7085,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>82</v>
       </c>
@@ -7102,7 +7102,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>83</v>
       </c>
@@ -7136,7 +7136,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -7153,7 +7153,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" ht="406" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -7187,7 +7187,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>88</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>89</v>
       </c>
@@ -7221,7 +7221,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>90</v>
       </c>
@@ -7238,7 +7238,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>91</v>
       </c>
@@ -7255,7 +7255,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>92</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>93</v>
       </c>
@@ -7289,7 +7289,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>94</v>
       </c>
@@ -7306,7 +7306,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>95</v>
       </c>
@@ -7323,7 +7323,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>96</v>
       </c>
@@ -7357,7 +7357,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="99" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>98</v>
       </c>
@@ -7374,7 +7374,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="100" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>99</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="102" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:5" ht="406" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>101</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="103" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>102</v>
       </c>
@@ -7442,7 +7442,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="104" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>103</v>
       </c>
@@ -7476,7 +7476,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="106" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>105</v>
       </c>
@@ -7493,7 +7493,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="107" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>106</v>
       </c>
@@ -7510,7 +7510,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="108" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>107</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>109</v>
       </c>
@@ -7561,7 +7561,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="111" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>110</v>
       </c>
@@ -7578,7 +7578,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="112" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
         <v>111</v>
       </c>
@@ -7612,7 +7612,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A114" s="2">
         <v>113</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A115" s="2">
         <v>114</v>
       </c>
@@ -7646,7 +7646,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="116" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A116" s="2">
         <v>115</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A118" s="2">
         <v>117</v>
       </c>
@@ -7731,7 +7731,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="121" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A121" s="2">
         <v>120</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A123" s="2">
         <v>122</v>
       </c>
@@ -7782,7 +7782,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="124" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A124" s="2">
         <v>123</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:5" ht="319" x14ac:dyDescent="0.35">
       <c r="A125" s="2">
         <v>124</v>
       </c>
@@ -7833,7 +7833,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="127" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
         <v>126</v>
       </c>
@@ -7850,7 +7850,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="128" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>127</v>
       </c>
@@ -7867,7 +7867,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A129" s="2">
         <v>128</v>
       </c>
@@ -7884,7 +7884,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="130" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A130" s="2">
         <v>129</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="131" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A131" s="2">
         <v>130</v>
       </c>
@@ -7918,7 +7918,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A132" s="2">
         <v>131</v>
       </c>
@@ -7952,7 +7952,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A134" s="2">
         <v>133</v>
       </c>
@@ -7969,7 +7969,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A135" s="2">
         <v>134</v>
       </c>
@@ -7986,7 +7986,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A136" s="2">
         <v>135</v>
       </c>
@@ -8003,7 +8003,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A137" s="2">
         <v>136</v>
       </c>
@@ -8020,7 +8020,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A138" s="2">
         <v>137</v>
       </c>
@@ -8037,7 +8037,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="139" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A139" s="2">
         <v>138</v>
       </c>
@@ -8139,7 +8139,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="145" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A145" s="2">
         <v>144</v>
       </c>
@@ -8156,7 +8156,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="146" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A146" s="2">
         <v>145</v>
       </c>
@@ -8190,7 +8190,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="148" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A148" s="2">
         <v>147</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="151" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A151" s="2">
         <v>150</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="152" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A152" s="2">
         <v>151</v>
       </c>
@@ -8292,7 +8292,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="154" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A154" s="2">
         <v>153</v>
       </c>
@@ -8309,7 +8309,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="155" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A155" s="2">
         <v>154</v>
       </c>
@@ -8326,7 +8326,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="156" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:5" ht="319" x14ac:dyDescent="0.35">
       <c r="A156" s="2">
         <v>155</v>
       </c>
@@ -8360,7 +8360,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="158" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A158" s="2">
         <v>157</v>
       </c>
@@ -8428,7 +8428,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="162" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A162" s="2">
         <v>161</v>
       </c>
@@ -8462,7 +8462,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="164" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A164" s="2">
         <v>163</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="165" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
       <c r="A165" s="2">
         <v>164</v>
       </c>
@@ -8496,7 +8496,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="166" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" ht="319" x14ac:dyDescent="0.35">
       <c r="A166" s="2">
         <v>165</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="167" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" ht="406" x14ac:dyDescent="0.35">
       <c r="A167" s="2">
         <v>166</v>
       </c>
@@ -8530,7 +8530,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="168" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A168" s="2">
         <v>167</v>
       </c>
@@ -8564,7 +8564,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="170" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" ht="348" x14ac:dyDescent="0.35">
       <c r="A170" s="2">
         <v>169</v>
       </c>
@@ -8581,7 +8581,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="171" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A171" s="2">
         <v>170</v>
       </c>
@@ -8598,7 +8598,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="172" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A172" s="2">
         <v>171</v>
       </c>
@@ -8615,7 +8615,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="173" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:5" ht="348" x14ac:dyDescent="0.35">
       <c r="A173" s="2">
         <v>172</v>
       </c>
@@ -8632,7 +8632,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="174" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A174" s="2">
         <v>173</v>
       </c>
@@ -8666,7 +8666,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="176" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A176" s="2">
         <v>175</v>
       </c>
@@ -8683,7 +8683,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="177" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A177" s="2">
         <v>176</v>
       </c>
@@ -8700,7 +8700,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="178" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A178" s="2">
         <v>177</v>
       </c>
@@ -8717,7 +8717,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="179" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A179" s="2">
         <v>178</v>
       </c>
@@ -8768,7 +8768,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="182" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:5" ht="319" x14ac:dyDescent="0.35">
       <c r="A182" s="2">
         <v>181</v>
       </c>
@@ -8785,7 +8785,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="183" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A183" s="2">
         <v>182</v>
       </c>
@@ -8819,7 +8819,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="185" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A185" s="2">
         <v>184</v>
       </c>
@@ -8836,7 +8836,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="186" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A186" s="2">
         <v>185</v>
       </c>
@@ -8853,7 +8853,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="187" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A187" s="2">
         <v>186</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="189" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
       <c r="A189" s="2">
         <v>188</v>
       </c>
@@ -8904,7 +8904,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="190" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A190" s="2">
         <v>189</v>
       </c>
@@ -8921,7 +8921,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="191" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A191" s="2">
         <v>190</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="192" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A192" s="2">
         <v>191</v>
       </c>
@@ -8955,7 +8955,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="193" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A193" s="2">
         <v>192</v>
       </c>
@@ -8972,7 +8972,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="194" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A194" s="2">
         <v>193</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="195" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A195" s="2">
         <v>194</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="196" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A196" s="2">
         <v>195</v>
       </c>
@@ -9023,7 +9023,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="197" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A197" s="2">
         <v>196</v>
       </c>
@@ -9040,7 +9040,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="198" spans="1:5" ht="232" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A198" s="2">
         <v>197</v>
       </c>
@@ -9057,7 +9057,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="199" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A199" s="2">
         <v>198</v>
       </c>
@@ -9074,7 +9074,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="200" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:5" ht="319" x14ac:dyDescent="0.35">
       <c r="A200" s="2">
         <v>199</v>
       </c>
@@ -9091,7 +9091,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="201" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A201" s="2">
         <v>200</v>
       </c>
@@ -9108,7 +9108,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="202" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A202" s="2">
         <v>201</v>
       </c>
@@ -9125,7 +9125,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="203" spans="1:5" ht="377" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:5" ht="348" x14ac:dyDescent="0.35">
       <c r="A203" s="2">
         <v>202</v>
       </c>
@@ -9142,7 +9142,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="204" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A204" s="2">
         <v>203</v>
       </c>
@@ -9159,7 +9159,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="205" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A205" s="2">
         <v>204</v>
       </c>
@@ -9176,7 +9176,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="206" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A206" s="2">
         <v>205</v>
       </c>
@@ -9244,7 +9244,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="210" spans="1:5" ht="290" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A210" s="2">
         <v>209</v>
       </c>
@@ -9295,7 +9295,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="213" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A213" s="2">
         <v>212</v>
       </c>
@@ -9312,7 +9312,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="214" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A214" s="2">
         <v>213</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="215" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A215" s="2">
         <v>214</v>
       </c>
@@ -9346,7 +9346,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="216" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A216" s="2">
         <v>215</v>
       </c>
@@ -9363,7 +9363,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="217" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A217" s="2">
         <v>216</v>
       </c>
@@ -9431,7 +9431,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="221" spans="1:5" ht="261" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A221" s="2">
         <v>220</v>
       </c>
@@ -9448,7 +9448,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="222" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A222" s="2">
         <v>221</v>
       </c>
@@ -9482,7 +9482,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="224" spans="1:5" ht="348" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A224" s="2">
         <v>223</v>
       </c>
@@ -9516,7 +9516,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="226" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:5" ht="406" x14ac:dyDescent="0.35">
       <c r="A226" s="2">
         <v>225</v>
       </c>
@@ -9533,7 +9533,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="227" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A227" s="2">
         <v>226</v>
       </c>
@@ -9567,7 +9567,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="229" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A229" s="2">
         <v>228</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="230" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A230" s="2">
         <v>229</v>
       </c>
@@ -9601,7 +9601,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="231" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A231" s="2">
         <v>230</v>
       </c>
@@ -9618,7 +9618,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="232" spans="1:5" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A232" s="2">
         <v>231</v>
       </c>
@@ -9652,7 +9652,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="234" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A234" s="2">
         <v>233</v>
       </c>
@@ -9669,7 +9669,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="235" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A235" s="2">
         <v>234</v>
       </c>
@@ -9686,7 +9686,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="236" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A236" s="2">
         <v>235</v>
       </c>
@@ -9720,7 +9720,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="238" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A238" s="2">
         <v>237</v>
       </c>
@@ -9754,7 +9754,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="240" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:5" ht="203" x14ac:dyDescent="0.35">
       <c r="A240" s="2">
         <v>239</v>
       </c>
@@ -9788,7 +9788,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="242" spans="1:5" ht="319" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A242" s="2">
         <v>241</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="243" spans="1:5" ht="391.5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A243" s="2">
         <v>242</v>
       </c>
@@ -9822,7 +9822,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="244" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A244" s="2">
         <v>243</v>
       </c>
@@ -9839,7 +9839,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="245" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:5" ht="232" x14ac:dyDescent="0.35">
       <c r="A245" s="2">
         <v>244</v>
       </c>
@@ -9856,7 +9856,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="246" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A246" s="2">
         <v>245</v>
       </c>
@@ -9873,7 +9873,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="247" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A247" s="2">
         <v>246</v>
       </c>
@@ -9924,7 +9924,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="250" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A250" s="2">
         <v>249</v>
       </c>
@@ -9941,7 +9941,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="251" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A251" s="2">
         <v>250</v>
       </c>
@@ -9975,7 +9975,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="253" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:5" ht="290" x14ac:dyDescent="0.35">
       <c r="A253" s="2">
         <v>252</v>
       </c>
@@ -9992,7 +9992,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="254" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A254" s="2">
         <v>253</v>
       </c>
@@ -10043,7 +10043,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="257" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A257" s="2">
         <v>256</v>
       </c>
@@ -10060,7 +10060,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="258" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A258" s="2">
         <v>257</v>
       </c>
@@ -10111,7 +10111,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="261" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A261" s="2">
         <v>260</v>
       </c>
@@ -10128,7 +10128,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="262" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A262" s="2">
         <v>261</v>
       </c>
@@ -10145,7 +10145,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="263" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A263" s="2">
         <v>262</v>
       </c>
@@ -10162,7 +10162,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="264" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:5" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A264" s="2">
         <v>263</v>
       </c>
@@ -10179,7 +10179,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="265" spans="1:5" ht="406" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:5" ht="377" x14ac:dyDescent="0.35">
       <c r="A265" s="2">
         <v>264</v>
       </c>
@@ -10196,7 +10196,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="266" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:5" ht="261" x14ac:dyDescent="0.35">
       <c r="A266" s="2">
         <v>265</v>
       </c>
@@ -10213,7 +10213,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="267" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A267" s="2">
         <v>266</v>
       </c>
@@ -10230,7 +10230,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="268" spans="1:5" ht="362.5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
       <c r="A268" s="2">
         <v>267</v>
       </c>
@@ -10247,7 +10247,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="269" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A269" s="2">
         <v>268</v>
       </c>
@@ -10264,7 +10264,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="270" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A270" s="2">
         <v>269</v>
       </c>
@@ -10281,7 +10281,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="271" spans="1:5" ht="203" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A271" s="2">
         <v>270</v>
       </c>
@@ -10332,7 +10332,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="274" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A274" s="2">
         <v>273</v>
       </c>
@@ -10366,7 +10366,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="276" spans="1:5" ht="333.5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:5" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A276" s="2">
         <v>275</v>
       </c>
@@ -10434,7 +10434,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="280" spans="1:5" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:5" ht="406" x14ac:dyDescent="0.35">
       <c r="A280" s="2">
         <v>279</v>
       </c>

</xml_diff>